<commit_message>
modify W10 and add W11
</commit_message>
<xml_diff>
--- a/Salary/W10 Salaries and Tasks.xlsx
+++ b/Salary/W10 Salaries and Tasks.xlsx
@@ -1,29 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11209"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jonas\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mina/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DCD151A6-8656-EA46-AF60-07B7653350F8}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9192" tabRatio="500"/>
+    <workbookView xWindow="19760" yWindow="3120" windowWidth="23040" windowHeight="9200" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913" concurrentCalc="0"/>
+  <calcPr calcId="181029" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="330"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-      </xcalcf:calcFeatures>
     </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -33,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
   <si>
     <t>Date</t>
   </si>
@@ -55,7 +50,7 @@
         <b/>
         <sz val="12"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="맑은 고딕"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -65,7 +60,7 @@
       <rPr>
         <sz val="12"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="맑은 고딕"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -78,7 +73,7 @@
         <b/>
         <sz val="12"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="맑은 고딕"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -88,7 +83,7 @@
       <rPr>
         <sz val="12"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="맑은 고딕"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -173,16 +168,24 @@
   <si>
     <t>Analyze our presentation feedback</t>
   </si>
+  <si>
+    <t>2019.11.14 - 2019.11.21</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>Present the User Study to stakeholders</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="6" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="7">
     <font>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="맑은 고딕"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -190,7 +193,7 @@
       <b/>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="맑은 고딕"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -218,6 +221,13 @@
       <color theme="1"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="맑은 고딕"/>
+      <family val="3"/>
+      <charset val="129"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="4">
@@ -324,7 +334,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="표준" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium7"/>
@@ -601,38 +611,38 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+    <sheetView tabSelected="1" topLeftCell="A14" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.796875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.85546875" defaultRowHeight="18"/>
   <cols>
-    <col min="1" max="1" width="36.19921875" customWidth="1"/>
-    <col min="2" max="2" width="34.69921875" customWidth="1"/>
+    <col min="1" max="1" width="36.140625" customWidth="1"/>
+    <col min="2" max="2" width="34.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="91.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" ht="91" customHeight="1">
       <c r="A1" s="9" t="s">
         <v>9</v>
       </c>
       <c r="B1" s="10"/>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2">
       <c r="A2" s="11"/>
       <c r="B2" s="11"/>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2">
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="2">
-        <v>43776</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B3" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
       <c r="A4" s="6" t="s">
         <v>1</v>
       </c>
@@ -640,7 +650,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2">
       <c r="A5" s="6" t="s">
         <v>2</v>
       </c>
@@ -648,11 +658,11 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2">
       <c r="A6" s="3"/>
       <c r="B6" s="4"/>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:2">
       <c r="A7" s="7" t="s">
         <v>6</v>
       </c>
@@ -660,7 +670,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:2">
       <c r="A8" s="7" t="s">
         <v>10</v>
       </c>
@@ -668,7 +678,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:2">
       <c r="A9" s="7" t="s">
         <v>11</v>
       </c>
@@ -676,7 +686,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:2">
       <c r="A10" s="7" t="s">
         <v>12</v>
       </c>
@@ -684,7 +694,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:2">
       <c r="A11" s="7" t="s">
         <v>13</v>
       </c>
@@ -692,7 +702,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:2">
       <c r="A12" s="7" t="s">
         <v>14</v>
       </c>
@@ -700,11 +710,11 @@
         <v>100</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:2">
       <c r="A13" s="4"/>
       <c r="B13" s="4"/>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:2">
       <c r="A14" s="6" t="s">
         <v>3</v>
       </c>
@@ -713,7 +723,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:2">
       <c r="A15" s="7" t="s">
         <v>5</v>
       </c>
@@ -722,15 +732,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:2">
       <c r="A16" s="4"/>
       <c r="B16" s="4"/>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:2">
       <c r="A17" s="4"/>
       <c r="B17" s="4"/>
     </row>
-    <row r="18" spans="1:2" ht="36.6" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:2" ht="41">
       <c r="A18" s="5" t="s">
         <v>7</v>
       </c>
@@ -738,7 +748,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:2">
       <c r="A19" s="7" t="s">
         <v>16</v>
       </c>
@@ -746,31 +756,33 @@
         <v>19</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:2">
       <c r="A20" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="B20" s="7"/>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B20" s="7" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2">
       <c r="A21" s="7" t="s">
         <v>18</v>
       </c>
       <c r="B21" s="7"/>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:2">
       <c r="A22" s="7"/>
       <c r="B22" s="7"/>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:2">
       <c r="A23" s="7"/>
       <c r="B23" s="7"/>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:2">
       <c r="A24" s="7"/>
       <c r="B24" s="7"/>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:2">
       <c r="A25" s="7"/>
       <c r="B25" s="7"/>
     </row>
@@ -779,6 +791,7 @@
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="A2:B2"/>
   </mergeCells>
+  <phoneticPr fontId="6" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>